<commit_message>
i have to find solution to Updating new scores Edits
</commit_message>
<xml_diff>
--- a/hominfoCSuper.xlsx
+++ b/hominfoCSuper.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\letenok\Documents\work\Flashscore\streaks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E25ACAA-6019-4EFD-86CE-2EC5A9EC3880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0533AC-D0A8-4A70-9FF0-29F9DB4A1785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -802,12 +802,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -837,11 +843,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1146,8 +1153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:EF17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AF11" sqref="AF11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1155,7 +1162,7 @@
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16.88671875" bestFit="1" customWidth="1"/>
@@ -1163,8 +1170,10 @@
     <col min="20" max="20" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="21" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="18" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="18" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="32" width="23.77734375" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="16" bestFit="1" customWidth="1"/>
@@ -5272,413 +5281,413 @@
         <v>155</v>
       </c>
     </row>
-    <row r="11" spans="1:136" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:136" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>12</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="L11" t="s">
+      <c r="L11" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="N11" t="s">
+      <c r="N11" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="O11" t="s">
+      <c r="O11" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="P11" t="s">
+      <c r="P11" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="Q11" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="R11" t="s">
+      <c r="R11" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="S11" t="s">
+      <c r="S11" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="T11" t="s">
+      <c r="T11" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="U11" t="s">
+      <c r="U11" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="V11" t="s">
+      <c r="V11" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="W11" t="s">
+      <c r="W11" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="X11" t="s">
+      <c r="X11" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="Y11" t="s">
+      <c r="Y11" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="Z11" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="AA11" t="s">
+      <c r="AA11" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AB11" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="AC11" t="s">
+      <c r="AC11" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="AD11" t="s">
+      <c r="AD11" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="AE11" t="s">
+      <c r="AE11" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="AF11" t="s">
+      <c r="AF11" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="AG11" t="s">
+      <c r="AG11" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="AH11" t="s">
+      <c r="AH11" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="AI11" t="s">
+      <c r="AI11" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="AJ11" t="s">
+      <c r="AJ11" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="AK11" t="s">
+      <c r="AK11" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="AL11" t="s">
+      <c r="AL11" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="AM11" t="s">
+      <c r="AM11" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="AN11" t="s">
+      <c r="AN11" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="AO11" t="s">
+      <c r="AO11" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="AP11" t="s">
+      <c r="AP11" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="AQ11" t="s">
+      <c r="AQ11" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="AR11" t="s">
+      <c r="AR11" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="AS11" t="s">
+      <c r="AS11" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="AT11" t="s">
-        <v>162</v>
-      </c>
-      <c r="AU11" t="s">
+      <c r="AT11" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AU11" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="AV11" t="s">
+      <c r="AV11" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="AW11" t="s">
+      <c r="AW11" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="AX11" t="s">
+      <c r="AX11" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="AY11" t="s">
+      <c r="AY11" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="AZ11" t="s">
+      <c r="AZ11" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="BA11" t="s">
-        <v>155</v>
-      </c>
-      <c r="BB11" t="s">
-        <v>155</v>
-      </c>
-      <c r="BC11" t="s">
-        <v>155</v>
-      </c>
-      <c r="BD11" t="s">
-        <v>155</v>
-      </c>
-      <c r="BE11" t="s">
-        <v>150</v>
-      </c>
-      <c r="BF11" t="s">
-        <v>150</v>
-      </c>
-      <c r="BG11" t="s">
-        <v>150</v>
-      </c>
-      <c r="BH11" t="s">
-        <v>150</v>
-      </c>
-      <c r="BI11" t="s">
+      <c r="BA11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="BB11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="BC11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="BD11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="BE11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="BF11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="BG11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="BH11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="BI11" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="BJ11" t="s">
+      <c r="BJ11" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="BK11" t="s">
+      <c r="BK11" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="BL11" t="s">
+      <c r="BL11" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="BM11" t="s">
+      <c r="BM11" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="BN11" t="s">
+      <c r="BN11" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="BO11" t="s">
+      <c r="BO11" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="BP11" t="s">
+      <c r="BP11" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="BQ11" t="s">
+      <c r="BQ11" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="BR11" t="s">
+      <c r="BR11" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="BS11" t="s">
+      <c r="BS11" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="BT11" t="s">
+      <c r="BT11" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="BU11" t="s">
-        <v>150</v>
-      </c>
-      <c r="BV11" t="s">
-        <v>165</v>
-      </c>
-      <c r="BW11" t="s">
-        <v>164</v>
-      </c>
-      <c r="BX11" t="s">
-        <v>164</v>
-      </c>
-      <c r="BY11" t="s">
-        <v>164</v>
-      </c>
-      <c r="BZ11" t="s">
-        <v>150</v>
-      </c>
-      <c r="CA11" t="s">
-        <v>150</v>
-      </c>
-      <c r="CB11" t="s">
-        <v>150</v>
-      </c>
-      <c r="CC11" t="s">
-        <v>150</v>
-      </c>
-      <c r="CD11" t="s">
-        <v>150</v>
-      </c>
-      <c r="CE11" t="s">
-        <v>150</v>
-      </c>
-      <c r="CF11" t="s">
-        <v>150</v>
-      </c>
-      <c r="CG11" t="s">
+      <c r="BU11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="BV11" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="BW11" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="BX11" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="BY11" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="BZ11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="CA11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="CB11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="CC11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="CD11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="CE11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="CF11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="CG11" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="CH11" t="s">
+      <c r="CH11" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="CI11" t="s">
+      <c r="CI11" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="CJ11" t="s">
+      <c r="CJ11" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="CK11" t="s">
-        <v>150</v>
-      </c>
-      <c r="CL11" t="s">
-        <v>150</v>
-      </c>
-      <c r="CM11" t="s">
-        <v>150</v>
-      </c>
-      <c r="CN11" t="s">
-        <v>150</v>
-      </c>
-      <c r="CO11" t="s">
-        <v>165</v>
-      </c>
-      <c r="CP11" t="s">
-        <v>165</v>
-      </c>
-      <c r="CQ11" t="s">
-        <v>165</v>
-      </c>
-      <c r="CR11" t="s">
-        <v>165</v>
-      </c>
-      <c r="CS11" t="s">
-        <v>150</v>
-      </c>
-      <c r="CT11" t="s">
-        <v>150</v>
-      </c>
-      <c r="CU11" t="s">
-        <v>150</v>
-      </c>
-      <c r="CV11" t="s">
-        <v>150</v>
-      </c>
-      <c r="CW11" t="s">
-        <v>150</v>
-      </c>
-      <c r="CX11" t="s">
-        <v>150</v>
-      </c>
-      <c r="CY11" t="s">
-        <v>150</v>
-      </c>
-      <c r="CZ11" t="s">
-        <v>162</v>
-      </c>
-      <c r="DA11" t="s">
+      <c r="CK11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="CL11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="CM11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="CN11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="CO11" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="CP11" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="CQ11" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="CR11" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="CS11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="CT11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="CU11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="CV11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="CW11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="CX11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="CY11" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="CZ11" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="DA11" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="DB11" t="s">
+      <c r="DB11" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="DC11" t="s">
+      <c r="DC11" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="DD11" t="s">
+      <c r="DD11" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="DE11" t="s">
+      <c r="DE11" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="DF11" t="s">
+      <c r="DF11" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="DG11" t="s">
+      <c r="DG11" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="DH11" t="s">
+      <c r="DH11" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="DI11" t="s">
-        <v>155</v>
-      </c>
-      <c r="DJ11" t="s">
-        <v>155</v>
-      </c>
-      <c r="DK11" t="s">
-        <v>155</v>
-      </c>
-      <c r="DL11" t="s">
-        <v>155</v>
-      </c>
-      <c r="DM11" t="s">
-        <v>155</v>
-      </c>
-      <c r="DN11" t="s">
-        <v>155</v>
-      </c>
-      <c r="DO11" t="s">
-        <v>155</v>
-      </c>
-      <c r="DP11" t="s">
-        <v>155</v>
-      </c>
-      <c r="DQ11" t="s">
+      <c r="DI11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="DJ11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="DK11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="DL11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="DM11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="DN11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="DO11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="DP11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="DQ11" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="DR11" t="s">
+      <c r="DR11" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="DS11" t="s">
+      <c r="DS11" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="DT11" t="s">
+      <c r="DT11" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="DU11" t="s">
+      <c r="DU11" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="DV11" t="s">
+      <c r="DV11" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="DW11" t="s">
+      <c r="DW11" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="DX11" t="s">
+      <c r="DX11" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="DY11" t="s">
-        <v>155</v>
-      </c>
-      <c r="DZ11" t="s">
-        <v>155</v>
-      </c>
-      <c r="EA11" t="s">
-        <v>155</v>
-      </c>
-      <c r="EB11" t="s">
-        <v>155</v>
-      </c>
-      <c r="EC11" t="s">
-        <v>155</v>
-      </c>
-      <c r="ED11" t="s">
-        <v>155</v>
-      </c>
-      <c r="EE11" t="s">
-        <v>155</v>
-      </c>
-      <c r="EF11" t="s">
+      <c r="DY11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="DZ11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="EA11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="EB11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="EC11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="ED11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="EE11" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="EF11" s="2" t="s">
         <v>155</v>
       </c>
     </row>

</xml_diff>